<commit_message>
created Rmarkdown and corrected minor unit issues and axis labels
</commit_message>
<xml_diff>
--- a/data/MI_traits_Est_by_Curtis.xlsx
+++ b/data/MI_traits_Est_by_Curtis.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10611"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/essing/Dropbox/Desktop/Rcode/Metabolic_Index/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/essing/Library/CloudStorage/Dropbox/Desktop/Rcode/Metabolic_Index/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E69781F3-13F3-4341-9020-B5B835320E8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{931FBD0D-99AC-D045-BE0C-881DBBBEFE89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="22620" windowHeight="25980" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -585,7 +585,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="allmidata_alphia"/>
@@ -7484,8 +7484,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F59" sqref="F59"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7566,19 +7567,19 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <f>LEN(A2)</f>
+        <f t="shared" ref="B2:B33" si="0">LEN(A2)</f>
         <v>29</v>
       </c>
       <c r="C2" t="str">
-        <f>RIGHT(A2,B2-5)</f>
+        <f t="shared" ref="C2:C33" si="1">RIGHT(A2,B2-5)</f>
         <v>Acanthephyra acutifrons'</v>
       </c>
       <c r="D2">
-        <f>LEN(C2)</f>
+        <f t="shared" ref="D2:D33" si="2">LEN(C2)</f>
         <v>24</v>
       </c>
       <c r="E2" t="str">
-        <f>LOWER(LEFT(C2,D2-1))</f>
+        <f t="shared" ref="E2:E12" si="3">LOWER(LEFT(C2,D2-1))</f>
         <v>acanthephyra acutifrons</v>
       </c>
       <c r="F2">
@@ -7635,19 +7636,19 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <f>LEN(A3)</f>
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="C3" t="str">
-        <f>RIGHT(A3,B3-5)</f>
+        <f t="shared" si="1"/>
         <v>Acanthephyra curtirostris'</v>
       </c>
       <c r="D3">
-        <f>LEN(C3)</f>
+        <f t="shared" si="2"/>
         <v>26</v>
       </c>
       <c r="E3" t="str">
-        <f>LOWER(LEFT(C3,D3-1))</f>
+        <f t="shared" si="3"/>
         <v>acanthephyra curtirostris</v>
       </c>
       <c r="F3" s="1">
@@ -7704,19 +7705,19 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <f>LEN(A4)</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="C4" t="str">
-        <f>RIGHT(A4,B4-5)</f>
+        <f t="shared" si="1"/>
         <v>Acanthephyra purpurea'</v>
       </c>
       <c r="D4">
-        <f>LEN(C4)</f>
+        <f t="shared" si="2"/>
         <v>22</v>
       </c>
       <c r="E4" t="str">
-        <f>LOWER(LEFT(C4,D4-1))</f>
+        <f t="shared" si="3"/>
         <v>acanthephyra purpurea</v>
       </c>
       <c r="F4">
@@ -7774,19 +7775,19 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <f>LEN(A5)</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="C5" t="str">
-        <f>RIGHT(A5,B5-5)</f>
+        <f t="shared" si="1"/>
         <v>Alitta succinea'</v>
       </c>
       <c r="D5">
-        <f>LEN(C5)</f>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="E5" t="str">
-        <f>LOWER(LEFT(C5,D5-1))</f>
+        <f t="shared" si="3"/>
         <v>alitta succinea</v>
       </c>
       <c r="F5">
@@ -7844,19 +7845,19 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <f>LEN(A6)</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="C6" t="str">
-        <f>RIGHT(A6,B6-5)</f>
+        <f t="shared" si="1"/>
         <v>Anguilla japonica'</v>
       </c>
       <c r="D6">
-        <f>LEN(C6)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="E6" t="str">
-        <f>LOWER(LEFT(C6,D6-1))</f>
+        <f t="shared" si="3"/>
         <v>anguilla japonica</v>
       </c>
       <c r="F6">
@@ -7914,19 +7915,19 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <f>LEN(A7)</f>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="C7" t="str">
-        <f>RIGHT(A7,B7-5)</f>
+        <f t="shared" si="1"/>
         <v>Bellapiscis lesleyae'</v>
       </c>
       <c r="D7">
-        <f>LEN(C7)</f>
+        <f t="shared" si="2"/>
         <v>21</v>
       </c>
       <c r="E7" t="str">
-        <f>LOWER(LEFT(C7,D7-1))</f>
+        <f t="shared" si="3"/>
         <v>bellapiscis lesleyae</v>
       </c>
       <c r="F7">
@@ -7984,19 +7985,19 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <f>LEN(A8)</f>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="C8" t="str">
-        <f>RIGHT(A8,B8-5)</f>
+        <f t="shared" si="1"/>
         <v>Bellapiscis medius'</v>
       </c>
       <c r="D8">
-        <f>LEN(C8)</f>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
       <c r="E8" t="str">
-        <f>LOWER(LEFT(C8,D8-1))</f>
+        <f t="shared" si="3"/>
         <v>bellapiscis medius</v>
       </c>
       <c r="F8">
@@ -8054,19 +8055,19 @@
         <v>17</v>
       </c>
       <c r="B9">
-        <f>LEN(A9)</f>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="C9" t="str">
-        <f>RIGHT(A9,B9-5)</f>
+        <f t="shared" si="1"/>
         <v>Cyclopterus lumpus'</v>
       </c>
       <c r="D9">
-        <f>LEN(C9)</f>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
       <c r="E9" t="str">
-        <f>LOWER(LEFT(C9,D9-1))</f>
+        <f t="shared" si="3"/>
         <v>cyclopterus lumpus</v>
       </c>
       <c r="F9">
@@ -8124,19 +8125,19 @@
         <v>20</v>
       </c>
       <c r="B10">
-        <f>LEN(A10)</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="C10" t="str">
-        <f>RIGHT(A10,B10-5)</f>
+        <f t="shared" si="1"/>
         <v>Doryteuthis pealeii'</v>
       </c>
       <c r="D10">
-        <f>LEN(C10)</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="E10" t="str">
-        <f>LOWER(LEFT(C10,D10-1))</f>
+        <f t="shared" si="3"/>
         <v>doryteuthis pealeii</v>
       </c>
       <c r="F10">
@@ -8194,19 +8195,19 @@
         <v>21</v>
       </c>
       <c r="B11">
-        <f>LEN(A11)</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="C11" t="str">
-        <f>RIGHT(A11,B11-5)</f>
+        <f t="shared" si="1"/>
         <v>Dosidicus gigas'</v>
       </c>
       <c r="D11">
-        <f>LEN(C11)</f>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="E11" t="str">
-        <f>LOWER(LEFT(C11,D11-1))</f>
+        <f t="shared" si="3"/>
         <v>dosidicus gigas</v>
       </c>
       <c r="F11">
@@ -8264,19 +8265,19 @@
         <v>22</v>
       </c>
       <c r="B12">
-        <f>LEN(A12)</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="C12" t="str">
-        <f>RIGHT(A12,B12-5)</f>
+        <f t="shared" si="1"/>
         <v>Funchalia villosa'</v>
       </c>
       <c r="D12">
-        <f>LEN(C12)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="E12" t="str">
-        <f>LOWER(LEFT(C12,D12-1))</f>
+        <f t="shared" si="3"/>
         <v>funchalia villosa</v>
       </c>
       <c r="F12">
@@ -8334,15 +8335,15 @@
         <v>25</v>
       </c>
       <c r="B13">
-        <f>LEN(A13)</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="C13" s="2" t="str">
-        <f>RIGHT(A13,B13-5)</f>
+        <f t="shared" si="1"/>
         <v>Gadus ogac'</v>
       </c>
       <c r="D13" s="2">
-        <f>LEN(C13)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="E13" s="2" t="s">
@@ -8403,15 +8404,15 @@
         <v>28</v>
       </c>
       <c r="B14">
-        <f>LEN(A14)</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="C14" t="str">
-        <f>RIGHT(A14,B14-5)</f>
+        <f t="shared" si="1"/>
         <v>Gennadas valens'</v>
       </c>
       <c r="D14">
-        <f>LEN(C14)</f>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="E14" t="str">
@@ -8473,15 +8474,15 @@
         <v>29</v>
       </c>
       <c r="B15">
-        <f>LEN(A15)</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="C15" t="str">
-        <f>RIGHT(A15,B15-5)</f>
+        <f t="shared" si="1"/>
         <v>Gibberulus gibbosus'</v>
       </c>
       <c r="D15">
-        <f>LEN(C15)</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="E15" t="str">
@@ -8543,15 +8544,15 @@
         <v>32</v>
       </c>
       <c r="B16">
-        <f>LEN(A16)</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="C16" s="2" t="str">
-        <f>RIGHT(A16,B16-5)</f>
+        <f t="shared" si="1"/>
         <v>Lophelia pertusa'</v>
       </c>
       <c r="D16" s="2">
-        <f>LEN(C16)</f>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="E16" s="2" t="s">
@@ -8612,15 +8613,15 @@
         <v>35</v>
       </c>
       <c r="B17">
-        <f>LEN(A17)</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="C17" t="str">
-        <f>RIGHT(A17,B17-5)</f>
+        <f t="shared" si="1"/>
         <v>Morone saxatilis'</v>
       </c>
       <c r="D17">
-        <f>LEN(C17)</f>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="E17" t="str">
@@ -8682,15 +8683,15 @@
         <v>38</v>
       </c>
       <c r="B18">
-        <f>LEN(A18)</f>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="C18" t="str">
-        <f>RIGHT(A18,B18-5)</f>
+        <f t="shared" si="1"/>
         <v>Notostomus elegans'</v>
       </c>
       <c r="D18">
-        <f>LEN(C18)</f>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
       <c r="E18" t="str">
@@ -8752,15 +8753,15 @@
         <v>39</v>
       </c>
       <c r="B19">
-        <f>LEN(A19)</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="C19" t="str">
-        <f>RIGHT(A19,B19-5)</f>
+        <f t="shared" si="1"/>
         <v>Notostomus gibbosus'</v>
       </c>
       <c r="D19">
-        <f>LEN(C19)</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="E19" t="str">
@@ -8822,15 +8823,15 @@
         <v>44</v>
       </c>
       <c r="B20">
-        <f>LEN(A20)</f>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="C20" t="str">
-        <f>RIGHT(A20,B20-5)</f>
+        <f t="shared" si="1"/>
         <v>Palaemonetes pugio'</v>
       </c>
       <c r="D20">
-        <f>LEN(C20)</f>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
       <c r="E20" t="s">
@@ -8891,19 +8892,19 @@
         <v>47</v>
       </c>
       <c r="B21">
-        <f>LEN(A21)</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="C21" t="str">
-        <f>RIGHT(A21,B21-5)</f>
+        <f t="shared" si="1"/>
         <v>Pandalus platyceros'</v>
       </c>
       <c r="D21">
-        <f>LEN(C21)</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="E21" t="str">
-        <f>LOWER(LEFT(C21,D21-1))</f>
+        <f t="shared" ref="E21:E27" si="4">LOWER(LEFT(C21,D21-1))</f>
         <v>pandalus platyceros</v>
       </c>
       <c r="F21">
@@ -8961,19 +8962,19 @@
         <v>49</v>
       </c>
       <c r="B22">
-        <f>LEN(A22)</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="C22" t="str">
-        <f>RIGHT(A22,B22-5)</f>
+        <f t="shared" si="1"/>
         <v>Panulirus interruptus'</v>
       </c>
       <c r="D22">
-        <f>LEN(C22)</f>
+        <f t="shared" si="2"/>
         <v>22</v>
       </c>
       <c r="E22" t="str">
-        <f>LOWER(LEFT(C22,D22-1))</f>
+        <f t="shared" si="4"/>
         <v>panulirus interruptus</v>
       </c>
       <c r="F22">
@@ -9031,19 +9032,19 @@
         <v>51</v>
       </c>
       <c r="B23">
-        <f>LEN(A23)</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="C23" t="str">
-        <f>RIGHT(A23,B23-5)</f>
+        <f t="shared" si="1"/>
         <v>Paralichthys dentatus'</v>
       </c>
       <c r="D23">
-        <f>LEN(C23)</f>
+        <f t="shared" si="2"/>
         <v>22</v>
       </c>
       <c r="E23" t="str">
-        <f>LOWER(LEFT(C23,D23-1))</f>
+        <f t="shared" si="4"/>
         <v>paralichthys dentatus</v>
       </c>
       <c r="F23">
@@ -9101,19 +9102,19 @@
         <v>53</v>
       </c>
       <c r="B24">
-        <f>LEN(A24)</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="C24" t="str">
-        <f>RIGHT(A24,B24-5)</f>
+        <f t="shared" si="1"/>
         <v>Penaeus aztecus'</v>
       </c>
       <c r="D24">
-        <f>LEN(C24)</f>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="E24" t="str">
-        <f>LOWER(LEFT(C24,D24-1))</f>
+        <f t="shared" si="4"/>
         <v>penaeus aztecus</v>
       </c>
       <c r="F24">
@@ -9171,19 +9172,19 @@
         <v>58</v>
       </c>
       <c r="B25">
-        <f>LEN(A25)</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="C25" t="str">
-        <f>RIGHT(A25,B25-5)</f>
+        <f t="shared" si="1"/>
         <v>Salpa fusiformis'</v>
       </c>
       <c r="D25">
-        <f>LEN(C25)</f>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="E25" t="str">
-        <f>LOWER(LEFT(C25,D25-1))</f>
+        <f t="shared" si="4"/>
         <v>salpa fusiformis</v>
       </c>
       <c r="F25">
@@ -9241,19 +9242,19 @@
         <v>59</v>
       </c>
       <c r="B26">
-        <f>LEN(A26)</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="C26" t="str">
-        <f>RIGHT(A26,B26-5)</f>
+        <f t="shared" si="1"/>
         <v>Sciaenops ocellatus'</v>
       </c>
       <c r="D26">
-        <f>LEN(C26)</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="E26" t="str">
-        <f>LOWER(LEFT(C26,D26-1))</f>
+        <f t="shared" si="4"/>
         <v>sciaenops ocellatus</v>
       </c>
       <c r="F26">
@@ -9311,19 +9312,19 @@
         <v>61</v>
       </c>
       <c r="B27">
-        <f>LEN(A27)</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="C27" t="str">
-        <f>RIGHT(A27,B27-5)</f>
+        <f t="shared" si="1"/>
         <v>Sepia officinalis'</v>
       </c>
       <c r="D27">
-        <f>LEN(C27)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="E27" t="str">
-        <f>LOWER(LEFT(C27,D27-1))</f>
+        <f t="shared" si="4"/>
         <v>sepia officinalis</v>
       </c>
       <c r="F27">
@@ -9381,15 +9382,15 @@
         <v>63</v>
       </c>
       <c r="B28">
-        <f>LEN(A28)</f>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="C28" t="str">
-        <f>RIGHT(A28,B28-5)</f>
+        <f t="shared" si="1"/>
         <v>Sergia grandis'</v>
       </c>
       <c r="D28">
-        <f>LEN(C28)</f>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="E28" t="s">
@@ -9450,19 +9451,19 @@
         <v>65</v>
       </c>
       <c r="B29">
-        <f>LEN(A29)</f>
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="C29" t="str">
-        <f>RIGHT(A29,B29-5)</f>
+        <f t="shared" si="1"/>
         <v>Stenobrachius leucopsarus'</v>
       </c>
       <c r="D29">
-        <f>LEN(C29)</f>
+        <f t="shared" si="2"/>
         <v>26</v>
       </c>
       <c r="E29" t="str">
-        <f>LOWER(LEFT(C29,D29-1))</f>
+        <f t="shared" ref="E29:E37" si="5">LOWER(LEFT(C29,D29-1))</f>
         <v>stenobrachius leucopsarus</v>
       </c>
       <c r="F29">
@@ -9520,19 +9521,19 @@
         <v>68</v>
       </c>
       <c r="B30">
-        <f>LEN(A30)</f>
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="C30" t="str">
-        <f>RIGHT(A30,B30-5)</f>
+        <f t="shared" si="1"/>
         <v>Tarletonbeania crenularis'</v>
       </c>
       <c r="D30">
-        <f>LEN(C30)</f>
+        <f t="shared" si="2"/>
         <v>26</v>
       </c>
       <c r="E30" t="str">
-        <f>LOWER(LEFT(C30,D30-1))</f>
+        <f t="shared" si="5"/>
         <v>tarletonbeania crenularis</v>
       </c>
       <c r="F30">
@@ -9590,19 +9591,19 @@
         <v>69</v>
       </c>
       <c r="B31">
-        <f>LEN(A31)</f>
+        <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="C31" t="str">
-        <f>RIGHT(A31,B31-5)</f>
+        <f t="shared" si="1"/>
         <v>Tautogolabrus adspersus'</v>
       </c>
       <c r="D31">
-        <f>LEN(C31)</f>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="E31" t="str">
-        <f>LOWER(LEFT(C31,D31-1))</f>
+        <f t="shared" si="5"/>
         <v>tautogolabrus adspersus</v>
       </c>
       <c r="F31">
@@ -9660,19 +9661,19 @@
         <v>70</v>
       </c>
       <c r="B32">
-        <f>LEN(A32)</f>
+        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="C32" t="str">
-        <f>RIGHT(A32,B32-5)</f>
+        <f t="shared" si="1"/>
         <v>Tigriopus brevicornis'</v>
       </c>
       <c r="D32">
-        <f>LEN(C32)</f>
+        <f t="shared" si="2"/>
         <v>22</v>
       </c>
       <c r="E32" t="str">
-        <f>LOWER(LEFT(C32,D32-1))</f>
+        <f t="shared" si="5"/>
         <v>tigriopus brevicornis</v>
       </c>
       <c r="F32">
@@ -9730,19 +9731,19 @@
         <v>3</v>
       </c>
       <c r="B33">
-        <f>LEN(A33)</f>
+        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="C33" t="str">
-        <f>RIGHT(A33,B33-5)</f>
+        <f t="shared" si="1"/>
         <v>Acanthephyra smithi'</v>
       </c>
       <c r="D33">
-        <f>LEN(C33)</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="E33" t="str">
-        <f>LOWER(LEFT(C33,D33-1))</f>
+        <f t="shared" si="5"/>
         <v>acanthephyra smithi</v>
       </c>
       <c r="F33">
@@ -9800,19 +9801,19 @@
         <v>9</v>
       </c>
       <c r="B34">
-        <f>LEN(A34)</f>
+        <f t="shared" ref="B34:B65" si="6">LEN(A34)</f>
         <v>27</v>
       </c>
       <c r="C34" t="str">
-        <f>RIGHT(A34,B34-5)</f>
+        <f t="shared" ref="C34:C65" si="7">RIGHT(A34,B34-5)</f>
         <v>Bythograea thermydron'</v>
       </c>
       <c r="D34">
-        <f>LEN(C34)</f>
+        <f t="shared" ref="D34:D65" si="8">LEN(C34)</f>
         <v>22</v>
       </c>
       <c r="E34" t="str">
-        <f>LOWER(LEFT(C34,D34-1))</f>
+        <f t="shared" si="5"/>
         <v>bythograea thermydron</v>
       </c>
       <c r="F34">
@@ -9870,19 +9871,19 @@
         <v>10</v>
       </c>
       <c r="B35">
-        <f>LEN(A35)</f>
+        <f t="shared" si="6"/>
         <v>25</v>
       </c>
       <c r="C35" t="str">
-        <f>RIGHT(A35,B35-5)</f>
+        <f t="shared" si="7"/>
         <v>Callinectes sapidus'</v>
       </c>
       <c r="D35">
-        <f>LEN(C35)</f>
+        <f t="shared" si="8"/>
         <v>20</v>
       </c>
       <c r="E35" t="str">
-        <f>LOWER(LEFT(C35,D35-1))</f>
+        <f t="shared" si="5"/>
         <v>callinectes sapidus</v>
       </c>
       <c r="F35">
@@ -9940,19 +9941,19 @@
         <v>12</v>
       </c>
       <c r="B36">
-        <f>LEN(A36)</f>
+        <f t="shared" si="6"/>
         <v>25</v>
       </c>
       <c r="C36" t="str">
-        <f>RIGHT(A36,B36-5)</f>
+        <f t="shared" si="7"/>
         <v>Carassius carassius'</v>
       </c>
       <c r="D36">
-        <f>LEN(C36)</f>
+        <f t="shared" si="8"/>
         <v>20</v>
       </c>
       <c r="E36" t="str">
-        <f>LOWER(LEFT(C36,D36-1))</f>
+        <f t="shared" si="5"/>
         <v>carassius carassius</v>
       </c>
       <c r="F36">
@@ -10010,19 +10011,19 @@
         <v>13</v>
       </c>
       <c r="B37">
-        <f>LEN(A37)</f>
+        <f t="shared" si="6"/>
         <v>21</v>
       </c>
       <c r="C37" t="str">
-        <f>RIGHT(A37,B37-5)</f>
+        <f t="shared" si="7"/>
         <v>Carcinus maenas'</v>
       </c>
       <c r="D37">
-        <f>LEN(C37)</f>
+        <f t="shared" si="8"/>
         <v>16</v>
       </c>
       <c r="E37" t="str">
-        <f>LOWER(LEFT(C37,D37-1))</f>
+        <f t="shared" si="5"/>
         <v>carcinus maenas</v>
       </c>
       <c r="F37">
@@ -10080,15 +10081,15 @@
         <v>16</v>
       </c>
       <c r="B38">
-        <f>LEN(A38)</f>
+        <f t="shared" si="6"/>
         <v>23</v>
       </c>
       <c r="C38" t="str">
-        <f>RIGHT(A38,B38-5)</f>
+        <f t="shared" si="7"/>
         <v>Crassostrea gigas'</v>
       </c>
       <c r="D38">
-        <f>LEN(C38)</f>
+        <f t="shared" si="8"/>
         <v>18</v>
       </c>
       <c r="E38" t="s">
@@ -10149,19 +10150,19 @@
         <v>24</v>
       </c>
       <c r="B39">
-        <f>LEN(A39)</f>
+        <f t="shared" si="6"/>
         <v>18</v>
       </c>
       <c r="C39" t="str">
-        <f>RIGHT(A39,B39-5)</f>
+        <f t="shared" si="7"/>
         <v>Gadus morhua'</v>
       </c>
       <c r="D39">
-        <f>LEN(C39)</f>
+        <f t="shared" si="8"/>
         <v>13</v>
       </c>
       <c r="E39" t="str">
-        <f>LOWER(LEFT(C39,D39-1))</f>
+        <f t="shared" ref="E39:E44" si="9">LOWER(LEFT(C39,D39-1))</f>
         <v>gadus morhua</v>
       </c>
       <c r="F39">
@@ -10219,19 +10220,19 @@
         <v>27</v>
       </c>
       <c r="B40">
-        <f>LEN(A40)</f>
+        <f t="shared" si="6"/>
         <v>22</v>
       </c>
       <c r="C40" t="str">
-        <f>RIGHT(A40,B40-5)</f>
+        <f t="shared" si="7"/>
         <v>Gaussia princeps'</v>
       </c>
       <c r="D40">
-        <f>LEN(C40)</f>
+        <f t="shared" si="8"/>
         <v>17</v>
       </c>
       <c r="E40" t="str">
-        <f>LOWER(LEFT(C40,D40-1))</f>
+        <f t="shared" si="9"/>
         <v>gaussia princeps</v>
       </c>
       <c r="F40">
@@ -10289,19 +10290,19 @@
         <v>36</v>
       </c>
       <c r="B41">
-        <f>LEN(A41)</f>
+        <f t="shared" si="6"/>
         <v>17</v>
       </c>
       <c r="C41" t="str">
-        <f>RIGHT(A41,B41-5)</f>
+        <f t="shared" si="7"/>
         <v>Mytilus sp.'</v>
       </c>
       <c r="D41">
-        <f>LEN(C41)</f>
+        <f t="shared" si="8"/>
         <v>12</v>
       </c>
       <c r="E41" t="str">
-        <f>LOWER(LEFT(C41,D41-1))</f>
+        <f t="shared" si="9"/>
         <v>mytilus sp.</v>
       </c>
       <c r="F41">
@@ -10359,19 +10360,19 @@
         <v>37</v>
       </c>
       <c r="B42">
-        <f>LEN(A42)</f>
+        <f t="shared" si="6"/>
         <v>24</v>
       </c>
       <c r="C42" t="str">
-        <f>RIGHT(A42,B42-5)</f>
+        <f t="shared" si="7"/>
         <v>Nautilus pompilius'</v>
       </c>
       <c r="D42">
-        <f>LEN(C42)</f>
+        <f t="shared" si="8"/>
         <v>19</v>
       </c>
       <c r="E42" t="str">
-        <f>LOWER(LEFT(C42,D42-1))</f>
+        <f t="shared" si="9"/>
         <v>nautilus pompilius</v>
       </c>
       <c r="F42">
@@ -10429,19 +10430,19 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <f>LEN(A43)</f>
+        <f t="shared" si="6"/>
         <v>31</v>
       </c>
       <c r="C43" t="str">
-        <f>RIGHT(A43,B43-5)</f>
+        <f t="shared" si="7"/>
         <v>Oplophorus gracilirostris'</v>
       </c>
       <c r="D43">
-        <f>LEN(C43)</f>
+        <f t="shared" si="8"/>
         <v>26</v>
       </c>
       <c r="E43" t="str">
-        <f>LOWER(LEFT(C43,D43-1))</f>
+        <f t="shared" si="9"/>
         <v>oplophorus gracilirostris</v>
       </c>
       <c r="F43">
@@ -10499,19 +10500,19 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <f>LEN(A44)</f>
+        <f t="shared" si="6"/>
         <v>25</v>
       </c>
       <c r="C44" t="str">
-        <f>RIGHT(A44,B44-5)</f>
+        <f t="shared" si="7"/>
         <v>Oplophorus spinosus'</v>
       </c>
       <c r="D44">
-        <f>LEN(C44)</f>
+        <f t="shared" si="8"/>
         <v>20</v>
       </c>
       <c r="E44" t="str">
-        <f>LOWER(LEFT(C44,D44-1))</f>
+        <f t="shared" si="9"/>
         <v>oplophorus spinosus</v>
       </c>
       <c r="F44">
@@ -10569,15 +10570,15 @@
         <v>45</v>
       </c>
       <c r="B45">
-        <f>LEN(A45)</f>
+        <f t="shared" si="6"/>
         <v>27</v>
       </c>
       <c r="C45" t="str">
-        <f>RIGHT(A45,B45-5)</f>
+        <f t="shared" si="7"/>
         <v>Palaemonetes vulgaris'</v>
       </c>
       <c r="D45">
-        <f>LEN(C45)</f>
+        <f t="shared" si="8"/>
         <v>22</v>
       </c>
       <c r="E45" t="s">
@@ -10638,15 +10639,15 @@
         <v>48</v>
       </c>
       <c r="B46">
-        <f>LEN(A46)</f>
+        <f t="shared" si="6"/>
         <v>22</v>
       </c>
       <c r="C46" t="str">
-        <f>RIGHT(A46,B46-5)</f>
+        <f t="shared" si="7"/>
         <v>Panulirus cygnus'</v>
       </c>
       <c r="D46">
-        <f>LEN(C46)</f>
+        <f t="shared" si="8"/>
         <v>17</v>
       </c>
       <c r="E46" t="str">
@@ -10708,15 +10709,15 @@
         <v>50</v>
       </c>
       <c r="B47">
-        <f>LEN(A47)</f>
+        <f t="shared" si="6"/>
         <v>27</v>
       </c>
       <c r="C47" t="str">
-        <f>RIGHT(A47,B47-5)</f>
+        <f t="shared" si="7"/>
         <v>Parabramis pekinensis'</v>
       </c>
       <c r="D47">
-        <f>LEN(C47)</f>
+        <f t="shared" si="8"/>
         <v>22</v>
       </c>
       <c r="E47" t="str">
@@ -10778,15 +10779,15 @@
         <v>52</v>
       </c>
       <c r="B48">
-        <f>LEN(A48)</f>
+        <f t="shared" si="6"/>
         <v>20</v>
       </c>
       <c r="C48" t="str">
-        <f>RIGHT(A48,B48-5)</f>
+        <f t="shared" si="7"/>
         <v>Pecten maximus'</v>
       </c>
       <c r="D48">
-        <f>LEN(C48)</f>
+        <f t="shared" si="8"/>
         <v>15</v>
       </c>
       <c r="E48" t="str">
@@ -10848,15 +10849,15 @@
         <v>55</v>
       </c>
       <c r="B49">
-        <f>LEN(A49)</f>
+        <f t="shared" si="6"/>
         <v>29</v>
       </c>
       <c r="C49" t="str">
-        <f>RIGHT(A49,B49-5)</f>
+        <f t="shared" si="7"/>
         <v>Phorgulsergia bisulcata'</v>
       </c>
       <c r="D49">
-        <f>LEN(C49)</f>
+        <f t="shared" si="8"/>
         <v>24</v>
       </c>
       <c r="E49" t="s">
@@ -10917,15 +10918,15 @@
         <v>60</v>
       </c>
       <c r="B50">
-        <f>LEN(A50)</f>
+        <f t="shared" si="6"/>
         <v>27</v>
       </c>
       <c r="C50" t="str">
-        <f>RIGHT(A50,B50-5)</f>
+        <f t="shared" si="7"/>
         <v>Scyliorhinus canicula'</v>
       </c>
       <c r="D50">
-        <f>LEN(C50)</f>
+        <f t="shared" si="8"/>
         <v>22</v>
       </c>
       <c r="E50" t="str">
@@ -10987,15 +10988,15 @@
         <v>62</v>
       </c>
       <c r="B51">
-        <f>LEN(A51)</f>
+        <f t="shared" si="6"/>
         <v>20</v>
       </c>
       <c r="C51" t="str">
-        <f>RIGHT(A51,B51-5)</f>
+        <f t="shared" si="7"/>
         <v>Sergia fulgens'</v>
       </c>
       <c r="D51">
-        <f>LEN(C51)</f>
+        <f t="shared" si="8"/>
         <v>15</v>
       </c>
       <c r="E51" t="s">
@@ -11056,19 +11057,19 @@
         <v>64</v>
       </c>
       <c r="B52">
-        <f>LEN(A52)</f>
+        <f t="shared" si="6"/>
         <v>23</v>
       </c>
       <c r="C52" t="str">
-        <f>RIGHT(A52,B52-5)</f>
+        <f t="shared" si="7"/>
         <v>Sergia tenuiremis'</v>
       </c>
       <c r="D52">
-        <f>LEN(C52)</f>
+        <f t="shared" si="8"/>
         <v>18</v>
       </c>
       <c r="E52" t="str">
-        <f>LOWER(LEFT(C52,D52-1))</f>
+        <f t="shared" ref="E52:E73" si="10">LOWER(LEFT(C52,D52-1))</f>
         <v>sergia tenuiremis</v>
       </c>
       <c r="F52">
@@ -11126,19 +11127,19 @@
         <v>30</v>
       </c>
       <c r="B53">
-        <f>LEN(A53)</f>
+        <f t="shared" si="6"/>
         <v>28</v>
       </c>
       <c r="C53" t="str">
-        <f>RIGHT(A53,B53-5)</f>
+        <f t="shared" si="7"/>
         <v>Gobiodon erythrospilus'</v>
       </c>
       <c r="D53">
-        <f>LEN(C53)</f>
+        <f t="shared" si="8"/>
         <v>23</v>
       </c>
       <c r="E53" t="str">
-        <f>LOWER(LEFT(C53,D53-1))</f>
+        <f t="shared" si="10"/>
         <v>gobiodon erythrospilus</v>
       </c>
       <c r="F53">
@@ -11196,19 +11197,19 @@
         <v>31</v>
       </c>
       <c r="B54">
-        <f>LEN(A54)</f>
+        <f t="shared" si="6"/>
         <v>22</v>
       </c>
       <c r="C54" t="str">
-        <f>RIGHT(A54,B54-5)</f>
+        <f t="shared" si="7"/>
         <v>Gobiodon histrio'</v>
       </c>
       <c r="D54">
-        <f>LEN(C54)</f>
+        <f t="shared" si="8"/>
         <v>17</v>
       </c>
       <c r="E54" t="str">
-        <f>LOWER(LEFT(C54,D54-1))</f>
+        <f t="shared" si="10"/>
         <v>gobiodon histrio</v>
       </c>
       <c r="F54">
@@ -11266,19 +11267,19 @@
         <v>34</v>
       </c>
       <c r="B55">
-        <f>LEN(A55)</f>
+        <f t="shared" si="6"/>
         <v>27</v>
       </c>
       <c r="C55" t="str">
-        <f>RIGHT(A55,B55-5)</f>
+        <f t="shared" si="7"/>
         <v>Melanostigma pammelas'</v>
       </c>
       <c r="D55">
-        <f>LEN(C55)</f>
+        <f t="shared" si="8"/>
         <v>22</v>
       </c>
       <c r="E55" t="str">
-        <f>LOWER(LEFT(C55,D55-1))</f>
+        <f t="shared" si="10"/>
         <v>melanostigma pammelas</v>
       </c>
       <c r="F55">
@@ -11336,19 +11337,19 @@
         <v>43</v>
       </c>
       <c r="B56">
-        <f>LEN(A56)</f>
+        <f t="shared" si="6"/>
         <v>27</v>
       </c>
       <c r="C56" t="str">
-        <f>RIGHT(A56,B56-5)</f>
+        <f t="shared" si="7"/>
         <v>Oreochromis niloticus'</v>
       </c>
       <c r="D56">
-        <f>LEN(C56)</f>
+        <f t="shared" si="8"/>
         <v>22</v>
       </c>
       <c r="E56" t="str">
-        <f>LOWER(LEFT(C56,D56-1))</f>
+        <f t="shared" si="10"/>
         <v>oreochromis niloticus</v>
       </c>
       <c r="F56">
@@ -11406,19 +11407,19 @@
         <v>46</v>
       </c>
       <c r="B57">
-        <f>LEN(A57)</f>
+        <f t="shared" si="6"/>
         <v>23</v>
       </c>
       <c r="C57" t="str">
-        <f>RIGHT(A57,B57-5)</f>
+        <f t="shared" si="7"/>
         <v>Pandalus borealis'</v>
       </c>
       <c r="D57">
-        <f>LEN(C57)</f>
+        <f t="shared" si="8"/>
         <v>18</v>
       </c>
       <c r="E57" t="str">
-        <f>LOWER(LEFT(C57,D57-1))</f>
+        <f t="shared" si="10"/>
         <v>pandalus borealis</v>
       </c>
       <c r="F57">
@@ -11476,19 +11477,19 @@
         <v>56</v>
       </c>
       <c r="B58">
-        <f>LEN(A58)</f>
+        <f t="shared" si="6"/>
         <v>27</v>
       </c>
       <c r="C58" t="str">
-        <f>RIGHT(A58,B58-5)</f>
+        <f t="shared" si="7"/>
         <v>Pleuroncodes planipes'</v>
       </c>
       <c r="D58">
-        <f>LEN(C58)</f>
+        <f t="shared" si="8"/>
         <v>22</v>
       </c>
       <c r="E58" t="str">
-        <f>LOWER(LEFT(C58,D58-1))</f>
+        <f t="shared" si="10"/>
         <v>pleuroncodes planipes</v>
       </c>
       <c r="F58">
@@ -11546,19 +11547,19 @@
         <v>57</v>
       </c>
       <c r="B59">
-        <f>LEN(A59)</f>
+        <f t="shared" si="6"/>
         <v>17</v>
       </c>
       <c r="C59" s="2" t="str">
-        <f>RIGHT(A59,B59-5)</f>
+        <f t="shared" si="7"/>
         <v>Salmo salar'</v>
       </c>
       <c r="D59" s="2">
-        <f>LEN(C59)</f>
+        <f t="shared" si="8"/>
         <v>12</v>
       </c>
       <c r="E59" s="2" t="str">
-        <f>LOWER(LEFT(C59,D59-1))</f>
+        <f t="shared" si="10"/>
         <v>salmo salar</v>
       </c>
       <c r="F59" s="1">
@@ -11615,19 +11616,19 @@
         <v>14</v>
       </c>
       <c r="B60">
-        <f>LEN(A60)</f>
+        <f t="shared" si="6"/>
         <v>27</v>
       </c>
       <c r="C60" t="str">
-        <f>RIGHT(A60,B60-5)</f>
+        <f t="shared" si="7"/>
         <v>Centropristis striata'</v>
       </c>
       <c r="D60">
-        <f>LEN(C60)</f>
+        <f t="shared" si="8"/>
         <v>22</v>
       </c>
       <c r="E60" t="str">
-        <f>LOWER(LEFT(C60,D60-1))</f>
+        <f t="shared" si="10"/>
         <v>centropristis striata</v>
       </c>
       <c r="F60">
@@ -11685,19 +11686,19 @@
         <v>71</v>
       </c>
       <c r="B61">
-        <f>LEN(A61)</f>
+        <f t="shared" si="6"/>
         <v>23</v>
       </c>
       <c r="C61" t="str">
-        <f>RIGHT(A61,B61-5)</f>
+        <f t="shared" si="7"/>
         <v>Zoarces viviparus'</v>
       </c>
       <c r="D61">
-        <f>LEN(C61)</f>
+        <f t="shared" si="8"/>
         <v>18</v>
       </c>
       <c r="E61" t="str">
-        <f>LOWER(LEFT(C61,D61-1))</f>
+        <f t="shared" si="10"/>
         <v>zoarces viviparus</v>
       </c>
       <c r="F61">
@@ -11755,19 +11756,19 @@
         <v>4</v>
       </c>
       <c r="B62">
-        <f>LEN(A62)</f>
+        <f t="shared" si="6"/>
         <v>28</v>
       </c>
       <c r="C62" t="str">
-        <f>RIGHT(A62,B62-5)</f>
+        <f t="shared" si="7"/>
         <v>Acipenser brevirostrum'</v>
       </c>
       <c r="D62">
-        <f>LEN(C62)</f>
+        <f t="shared" si="8"/>
         <v>23</v>
       </c>
       <c r="E62" t="str">
-        <f>LOWER(LEFT(C62,D62-1))</f>
+        <f t="shared" si="10"/>
         <v>acipenser brevirostrum</v>
       </c>
       <c r="F62">
@@ -11825,19 +11826,19 @@
         <v>23</v>
       </c>
       <c r="B63">
-        <f>LEN(A63)</f>
+        <f t="shared" si="6"/>
         <v>18</v>
       </c>
       <c r="C63" t="str">
-        <f>RIGHT(A63,B63-5)</f>
+        <f t="shared" si="7"/>
         <v>Gadus Morhua'</v>
       </c>
       <c r="D63">
-        <f>LEN(C63)</f>
+        <f t="shared" si="8"/>
         <v>13</v>
       </c>
       <c r="E63" t="str">
-        <f>LOWER(LEFT(C63,D63-1))</f>
+        <f t="shared" si="10"/>
         <v>gadus morhua</v>
       </c>
       <c r="F63">
@@ -11895,19 +11896,19 @@
         <v>67</v>
       </c>
       <c r="B64">
-        <f>LEN(A64)</f>
+        <f t="shared" si="6"/>
         <v>26</v>
       </c>
       <c r="C64" t="str">
-        <f>RIGHT(A64,B64-5)</f>
+        <f t="shared" si="7"/>
         <v>Systellaspis debilis'</v>
       </c>
       <c r="D64">
-        <f>LEN(C64)</f>
+        <f t="shared" si="8"/>
         <v>21</v>
       </c>
       <c r="E64" t="str">
-        <f>LOWER(LEFT(C64,D64-1))</f>
+        <f t="shared" si="10"/>
         <v>systellaspis debilis</v>
       </c>
       <c r="F64">
@@ -11965,19 +11966,19 @@
         <v>54</v>
       </c>
       <c r="B65">
-        <f>LEN(A65)</f>
+        <f t="shared" si="6"/>
         <v>22</v>
       </c>
       <c r="C65" t="str">
-        <f>RIGHT(A65,B65-5)</f>
+        <f t="shared" si="7"/>
         <v>Penaeus vannamei'</v>
       </c>
       <c r="D65">
-        <f>LEN(C65)</f>
+        <f t="shared" si="8"/>
         <v>17</v>
       </c>
       <c r="E65" t="str">
-        <f>LOWER(LEFT(C65,D65-1))</f>
+        <f t="shared" si="10"/>
         <v>penaeus vannamei</v>
       </c>
       <c r="F65">
@@ -12035,19 +12036,19 @@
         <v>66</v>
       </c>
       <c r="B66">
-        <f>LEN(A66)</f>
+        <f t="shared" ref="B66:B73" si="11">LEN(A66)</f>
         <v>20</v>
       </c>
       <c r="C66" t="str">
-        <f>RIGHT(A66,B66-5)</f>
+        <f t="shared" ref="C66:C73" si="12">RIGHT(A66,B66-5)</f>
         <v>Styela plicata'</v>
       </c>
       <c r="D66">
-        <f>LEN(C66)</f>
+        <f t="shared" ref="D66:D73" si="13">LEN(C66)</f>
         <v>15</v>
       </c>
       <c r="E66" t="str">
-        <f>LOWER(LEFT(C66,D66-1))</f>
+        <f t="shared" si="10"/>
         <v>styela plicata</v>
       </c>
       <c r="F66">
@@ -12105,19 +12106,19 @@
         <v>18</v>
       </c>
       <c r="B67">
-        <f>LEN(A67)</f>
+        <f t="shared" si="11"/>
         <v>19</v>
       </c>
       <c r="C67" t="str">
-        <f>RIGHT(A67,B67-5)</f>
+        <f t="shared" si="12"/>
         <v>Dentex dentex'</v>
       </c>
       <c r="D67">
-        <f>LEN(C67)</f>
+        <f t="shared" si="13"/>
         <v>14</v>
       </c>
       <c r="E67" t="str">
-        <f>LOWER(LEFT(C67,D67-1))</f>
+        <f t="shared" si="10"/>
         <v>dentex dentex</v>
       </c>
       <c r="F67">
@@ -12175,19 +12176,19 @@
         <v>19</v>
       </c>
       <c r="B68">
-        <f>LEN(A68)</f>
+        <f t="shared" si="11"/>
         <v>23</v>
       </c>
       <c r="C68" t="str">
-        <f>RIGHT(A68,B68-5)</f>
+        <f t="shared" si="12"/>
         <v>Diplodus puntazzo'</v>
       </c>
       <c r="D68">
-        <f>LEN(C68)</f>
+        <f t="shared" si="13"/>
         <v>18</v>
       </c>
       <c r="E68" t="str">
-        <f>LOWER(LEFT(C68,D68-1))</f>
+        <f t="shared" si="10"/>
         <v>diplodus puntazzo</v>
       </c>
       <c r="F68">
@@ -12245,19 +12246,19 @@
         <v>33</v>
       </c>
       <c r="B69">
-        <f>LEN(A69)</f>
+        <f t="shared" si="11"/>
         <v>24</v>
       </c>
       <c r="C69" t="str">
-        <f>RIGHT(A69,B69-5)</f>
+        <f t="shared" si="12"/>
         <v>Maja brachydactyla'</v>
       </c>
       <c r="D69">
-        <f>LEN(C69)</f>
+        <f t="shared" si="13"/>
         <v>19</v>
       </c>
       <c r="E69" t="str">
-        <f>LOWER(LEFT(C69,D69-1))</f>
+        <f t="shared" si="10"/>
         <v>maja brachydactyla</v>
       </c>
       <c r="F69">
@@ -12315,19 +12316,19 @@
         <v>40</v>
       </c>
       <c r="B70">
-        <f>LEN(A70)</f>
+        <f t="shared" si="11"/>
         <v>22</v>
       </c>
       <c r="C70" t="str">
-        <f>RIGHT(A70,B70-5)</f>
+        <f t="shared" si="12"/>
         <v>Octopus vulgaris'</v>
       </c>
       <c r="D70">
-        <f>LEN(C70)</f>
+        <f t="shared" si="13"/>
         <v>17</v>
       </c>
       <c r="E70" t="str">
-        <f>LOWER(LEFT(C70,D70-1))</f>
+        <f t="shared" si="10"/>
         <v>octopus vulgaris</v>
       </c>
       <c r="F70">
@@ -12385,19 +12386,19 @@
         <v>26</v>
       </c>
       <c r="B71">
-        <f>LEN(A71)</f>
+        <f t="shared" si="11"/>
         <v>29</v>
       </c>
       <c r="C71" t="str">
-        <f>RIGHT(A71,B71-5)</f>
+        <f t="shared" si="12"/>
         <v>Gammarus pseudolimnaeus'</v>
       </c>
       <c r="D71">
-        <f>LEN(C71)</f>
+        <f t="shared" si="13"/>
         <v>24</v>
       </c>
       <c r="E71" t="str">
-        <f>LOWER(LEFT(C71,D71-1))</f>
+        <f t="shared" si="10"/>
         <v>gammarus pseudolimnaeus</v>
       </c>
       <c r="F71">
@@ -12455,19 +12456,19 @@
         <v>15</v>
       </c>
       <c r="B72">
-        <f>LEN(A72)</f>
+        <f t="shared" si="11"/>
         <v>28</v>
       </c>
       <c r="C72" t="str">
-        <f>RIGHT(A72,B72-5)</f>
+        <f t="shared" si="12"/>
         <v>Chromis atripectoralis'</v>
       </c>
       <c r="D72">
-        <f>LEN(C72)</f>
+        <f t="shared" si="13"/>
         <v>23</v>
       </c>
       <c r="E72" t="str">
-        <f>LOWER(LEFT(C72,D72-1))</f>
+        <f t="shared" si="10"/>
         <v>chromis atripectoralis</v>
       </c>
       <c r="F72">
@@ -12525,19 +12526,19 @@
         <v>11</v>
       </c>
       <c r="B73">
-        <f>LEN(A73)</f>
+        <f t="shared" si="11"/>
         <v>22</v>
       </c>
       <c r="C73" t="str">
-        <f>RIGHT(A73,B73-5)</f>
+        <f t="shared" si="12"/>
         <v>Cancer irroratus'</v>
       </c>
       <c r="D73">
-        <f>LEN(C73)</f>
+        <f t="shared" si="13"/>
         <v>17</v>
       </c>
       <c r="E73" t="str">
-        <f>LOWER(LEFT(C73,D73-1))</f>
+        <f t="shared" si="10"/>
         <v>cancer irroratus</v>
       </c>
       <c r="F73">

</xml_diff>